<commit_message>
climate driver look up
</commit_message>
<xml_diff>
--- a/data_cleaning/otherclimatedrivers_lookup.xlsx
+++ b/data_cleaning/otherclimatedrivers_lookup.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annalopresti/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://o365coloradoedu-my.sharepoint.com/personal/lade8828_colorado_edu/Documents/Documents/GitHub/BCCAch7/data_cleaning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{375ABBDB-2172-CD4B-A68F-09F2D9E2886E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{375ABBDB-2172-CD4B-A68F-09F2D9E2886E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E4B19AE5-9F94-2241-8167-89C5EA263304}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="520" windowWidth="14380" windowHeight="16440" activeTab="1" xr2:uid="{2621AD7F-AB1A-E74A-BB38-AD63999953F2}"/>
+    <workbookView xWindow="1560" yWindow="760" windowWidth="15500" windowHeight="16440" xr2:uid="{2621AD7F-AB1A-E74A-BB38-AD63999953F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="67">
   <si>
     <t>raw</t>
   </si>
@@ -235,6 +235,9 @@
   </si>
   <si>
     <t>sub-category</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -614,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F8994F6-F41D-6944-BEB6-66E836A5D57A}">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -768,6 +771,9 @@
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="B17" t="s">
+        <v>66</v>
+      </c>
       <c r="C17" t="s">
         <v>42</v>
       </c>
@@ -776,6 +782,9 @@
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="B18" t="s">
+        <v>66</v>
+      </c>
       <c r="C18" t="s">
         <v>42</v>
       </c>
@@ -784,6 +793,9 @@
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="B19" t="s">
+        <v>66</v>
+      </c>
       <c r="C19" t="s">
         <v>42</v>
       </c>
@@ -811,6 +823,9 @@
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="B22" t="s">
+        <v>66</v>
+      </c>
       <c r="C22" t="s">
         <v>42</v>
       </c>
@@ -818,6 +833,9 @@
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>23</v>
+      </c>
+      <c r="B23" t="s">
+        <v>66</v>
       </c>
       <c r="C23" t="s">
         <v>42</v>
@@ -944,8 +962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F89E10-CA8D-FC46-9106-B1361C4EBA63}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>